<commit_message>
LIvro.xlsl commit due to pull
</commit_message>
<xml_diff>
--- a/Livro1.xlsx
+++ b/Livro1.xlsx
@@ -80,9 +80,6 @@
     <t>https://www.robotshop.com/eu/en/pololu-micro-mounting-bracket-extended.html</t>
   </si>
   <si>
-    <t>https://www.robotshop.com/eu/en/drv8835-dual-motor-driver-carrier.html</t>
-  </si>
-  <si>
     <t>https://www.robotshop.com/eu/en/tof-range-finder-sensor-breakout-board-voltage-regulator-vl53l0x.html</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>shipping</t>
+  </si>
+  <si>
+    <t>https://www.robotshop.com/eu/en/pololu-drv8833-motor-controller-2130.html</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +547,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <f>C5*B5</f>
+        <f t="shared" ref="D5:D24" si="1">C5*B5</f>
         <v>7.2</v>
       </c>
       <c r="E5" t="s">
@@ -568,14 +568,14 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <f>C6*B6</f>
+        <f t="shared" si="1"/>
         <v>4.53</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -589,7 +589,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f>C7*B7</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E7" t="s">
@@ -610,32 +610,32 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <f>C8*B8</f>
+        <f t="shared" si="1"/>
         <v>30.06</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9">
-        <f>C9*B9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10">
-        <f>C10*B10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D11">
-        <f>C11*B11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O11">
         <f>D1</f>
@@ -644,11 +644,11 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12">
-        <f>C12*B12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O12">
         <v>13.12</v>
@@ -656,11 +656,11 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D13">
-        <f>C13*B13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O13">
         <f>SUM(O11:O12)</f>
@@ -669,67 +669,67 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14">
-        <f>C14*B14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15">
-        <f>C15*B15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16">
-        <f>C16*B16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
-        <f>C17*B17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18">
-        <f>C18*B18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19">
-        <f>C19*B19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20">
-        <f>C20*B20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21">
-        <f>C21*B21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22">
-        <f>C22*B22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23">
-        <f>C23*B23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24">
-        <f>C24*B24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>